<commit_message>
Thêm hiển thị mã nhân viên , chỉnh sử excel template
thêm mã nhân viên cho bảng chứng chỉ của nhân viên và bảng bằng cấp-giấy chứng nhận của nhân viên . Chỉnh sửa excel bảng bằng cấp( thêm hiển thị)
</commit_message>
<xml_diff>
--- a/QUANGHANH2/excel/TCLD/Diploma/bằng cấp và giấy chứng nhận của nhân viên.xlsx
+++ b/QUANGHANH2/excel/TCLD/Diploma/bằng cấp và giấy chứng nhận của nhân viên.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Số hiệu</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>STT</t>
+  </si>
+  <si>
+    <t>Mã nhân viên</t>
   </si>
 </sst>
 </file>
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -425,12 +428,13 @@
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="16.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="31.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="19.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="25.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="25.2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -438,8 +442,9 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -450,15 +455,18 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>